<commit_message>
Upload Y4_B2526_General_Surgery_checklist1758105464464_backup@backdoor.com.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_General_Surgery_checklist1758105464464_backup@backdoor.com.xlsx
+++ b/log_history/Y4_B2526_General_Surgery_checklist1758105464464_backup@backdoor.com.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\log_history\Imported_logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\log_history\Imported_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E0DF50-67EF-4E21-9D03-A2C716AC9CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="2280" yWindow="1300" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -258,10 +259,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="h:mm:ss;@"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -291,11 +289,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,26 +631,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D69"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.875" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.25" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -666,7 +664,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -674,7 +672,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1">
-        <v>45817</v>
+        <v>45906</v>
       </c>
       <c r="D2" s="2">
         <v>0.48561342592592593</v>
@@ -686,7 +684,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -694,9 +692,9 @@
         <v>7</v>
       </c>
       <c r="C3" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D3" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D3" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E3" t="s">
@@ -706,7 +704,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -714,9 +712,9 @@
         <v>7</v>
       </c>
       <c r="C4" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D4" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D4" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E4" t="s">
@@ -726,7 +724,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -734,9 +732,9 @@
         <v>7</v>
       </c>
       <c r="C5" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D5" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D5" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E5" t="s">
@@ -746,7 +744,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -754,9 +752,9 @@
         <v>7</v>
       </c>
       <c r="C6" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D6" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D6" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E6" t="s">
@@ -766,7 +764,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -774,9 +772,9 @@
         <v>7</v>
       </c>
       <c r="C7" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D7" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D7" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E7" t="s">
@@ -786,7 +784,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -794,9 +792,9 @@
         <v>7</v>
       </c>
       <c r="C8" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D8" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D8" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E8" t="s">
@@ -806,7 +804,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -814,9 +812,9 @@
         <v>7</v>
       </c>
       <c r="C9" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D9" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D9" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E9" t="s">
@@ -826,7 +824,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -834,9 +832,9 @@
         <v>7</v>
       </c>
       <c r="C10" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D10" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D10" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E10" t="s">
@@ -846,7 +844,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -854,9 +852,9 @@
         <v>7</v>
       </c>
       <c r="C11" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D11" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D11" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E11" t="s">
@@ -866,7 +864,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -874,9 +872,9 @@
         <v>7</v>
       </c>
       <c r="C12" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D12" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D12" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E12" t="s">
@@ -886,7 +884,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -894,9 +892,9 @@
         <v>7</v>
       </c>
       <c r="C13" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D13" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D13" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E13" t="s">
@@ -906,7 +904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -914,9 +912,9 @@
         <v>7</v>
       </c>
       <c r="C14" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D14" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D14" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E14" t="s">
@@ -926,7 +924,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -934,9 +932,9 @@
         <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D15" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D15" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E15" t="s">
@@ -946,7 +944,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -954,9 +952,9 @@
         <v>7</v>
       </c>
       <c r="C16" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D16" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D16" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E16" t="s">
@@ -966,7 +964,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -974,9 +972,9 @@
         <v>7</v>
       </c>
       <c r="C17" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D17" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D17" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E17" t="s">
@@ -986,7 +984,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -994,9 +992,9 @@
         <v>7</v>
       </c>
       <c r="C18" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D18" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D18" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E18" t="s">
@@ -1006,7 +1004,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1014,9 +1012,9 @@
         <v>7</v>
       </c>
       <c r="C19" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D19" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D19" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E19" t="s">
@@ -1026,7 +1024,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1034,9 +1032,9 @@
         <v>7</v>
       </c>
       <c r="C20" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D20" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D20" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E20" t="s">
@@ -1046,7 +1044,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1054,9 +1052,9 @@
         <v>7</v>
       </c>
       <c r="C21" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D21" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D21" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E21" t="s">
@@ -1066,7 +1064,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1074,9 +1072,9 @@
         <v>7</v>
       </c>
       <c r="C22" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D22" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D22" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E22" t="s">
@@ -1086,7 +1084,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -1094,9 +1092,9 @@
         <v>7</v>
       </c>
       <c r="C23" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D23" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D23" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E23" t="s">
@@ -1106,7 +1104,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -1114,9 +1112,9 @@
         <v>7</v>
       </c>
       <c r="C24" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D24" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D24" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E24" t="s">
@@ -1126,7 +1124,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1134,9 +1132,9 @@
         <v>7</v>
       </c>
       <c r="C25" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D25" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D25" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E25" t="s">
@@ -1146,7 +1144,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1154,9 +1152,9 @@
         <v>7</v>
       </c>
       <c r="C26" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D26" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D26" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E26" t="s">
@@ -1166,7 +1164,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1174,9 +1172,9 @@
         <v>7</v>
       </c>
       <c r="C27" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D27" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D27" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E27" t="s">
@@ -1186,7 +1184,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -1194,9 +1192,9 @@
         <v>7</v>
       </c>
       <c r="C28" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D28" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D28" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E28" t="s">
@@ -1206,7 +1204,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -1214,9 +1212,9 @@
         <v>7</v>
       </c>
       <c r="C29" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D29" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D29" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E29" t="s">
@@ -1226,7 +1224,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -1234,9 +1232,9 @@
         <v>7</v>
       </c>
       <c r="C30" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D30" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D30" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E30" t="s">
@@ -1246,7 +1244,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -1254,9 +1252,9 @@
         <v>7</v>
       </c>
       <c r="C31" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D31" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D31" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E31" t="s">
@@ -1266,7 +1264,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -1274,9 +1272,9 @@
         <v>7</v>
       </c>
       <c r="C32" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D32" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D32" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E32" t="s">
@@ -1286,7 +1284,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -1294,9 +1292,9 @@
         <v>7</v>
       </c>
       <c r="C33" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D33" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D33" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E33" t="s">
@@ -1306,7 +1304,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -1314,9 +1312,9 @@
         <v>7</v>
       </c>
       <c r="C34" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D34" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D34" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E34" t="s">
@@ -1326,7 +1324,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -1334,9 +1332,9 @@
         <v>7</v>
       </c>
       <c r="C35" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D35" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D35" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E35" t="s">
@@ -1346,7 +1344,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -1354,9 +1352,9 @@
         <v>7</v>
       </c>
       <c r="C36" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D36" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D36" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E36" t="s">
@@ -1366,7 +1364,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -1374,9 +1372,9 @@
         <v>7</v>
       </c>
       <c r="C37" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D37" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D37" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E37" t="s">
@@ -1386,7 +1384,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -1394,9 +1392,9 @@
         <v>7</v>
       </c>
       <c r="C38" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D38" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D38" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E38" t="s">
@@ -1406,7 +1404,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -1414,9 +1412,9 @@
         <v>7</v>
       </c>
       <c r="C39" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D39" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D39" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E39" t="s">
@@ -1426,7 +1424,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -1434,9 +1432,9 @@
         <v>7</v>
       </c>
       <c r="C40" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D40" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D40" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E40" t="s">
@@ -1446,7 +1444,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -1454,9 +1452,9 @@
         <v>7</v>
       </c>
       <c r="C41" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D41" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D41" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E41" t="s">
@@ -1466,7 +1464,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -1474,9 +1472,9 @@
         <v>7</v>
       </c>
       <c r="C42" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D42" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D42" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E42" t="s">
@@ -1486,7 +1484,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -1494,9 +1492,9 @@
         <v>7</v>
       </c>
       <c r="C43" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D43" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D43" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E43" t="s">
@@ -1506,7 +1504,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -1514,9 +1512,9 @@
         <v>7</v>
       </c>
       <c r="C44" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D44" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D44" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E44" t="s">
@@ -1526,7 +1524,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -1534,9 +1532,9 @@
         <v>7</v>
       </c>
       <c r="C45" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D45" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D45" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E45" t="s">
@@ -1546,7 +1544,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>54</v>
       </c>
@@ -1554,9 +1552,9 @@
         <v>7</v>
       </c>
       <c r="C46" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D46" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D46" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E46" t="s">
@@ -1566,7 +1564,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -1574,9 +1572,9 @@
         <v>7</v>
       </c>
       <c r="C47" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D47" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D47" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E47" t="s">
@@ -1586,7 +1584,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -1594,9 +1592,9 @@
         <v>7</v>
       </c>
       <c r="C48" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D48" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D48" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E48" t="s">
@@ -1606,7 +1604,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -1614,9 +1612,9 @@
         <v>7</v>
       </c>
       <c r="C49" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D49" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D49" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E49" t="s">
@@ -1626,7 +1624,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -1634,9 +1632,9 @@
         <v>7</v>
       </c>
       <c r="C50" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D50" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D50" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E50" t="s">
@@ -1646,7 +1644,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -1654,9 +1652,9 @@
         <v>7</v>
       </c>
       <c r="C51" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D51" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D51" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E51" t="s">
@@ -1666,7 +1664,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -1674,9 +1672,9 @@
         <v>7</v>
       </c>
       <c r="C52" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D52" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D52" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E52" t="s">
@@ -1686,7 +1684,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>61</v>
       </c>
@@ -1694,9 +1692,9 @@
         <v>7</v>
       </c>
       <c r="C53" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D53" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D53" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E53" t="s">
@@ -1706,7 +1704,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>62</v>
       </c>
@@ -1714,9 +1712,9 @@
         <v>7</v>
       </c>
       <c r="C54" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D54" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D54" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E54" t="s">
@@ -1726,7 +1724,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>63</v>
       </c>
@@ -1734,9 +1732,9 @@
         <v>7</v>
       </c>
       <c r="C55" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D55" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D55" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E55" t="s">
@@ -1746,7 +1744,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>64</v>
       </c>
@@ -1754,9 +1752,9 @@
         <v>7</v>
       </c>
       <c r="C56" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D56" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D56" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E56" t="s">
@@ -1766,7 +1764,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>65</v>
       </c>
@@ -1774,9 +1772,9 @@
         <v>7</v>
       </c>
       <c r="C57" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D57" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D57" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E57" t="s">
@@ -1786,7 +1784,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>66</v>
       </c>
@@ -1794,9 +1792,9 @@
         <v>7</v>
       </c>
       <c r="C58" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D58" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D58" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E58" t="s">
@@ -1806,7 +1804,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>67</v>
       </c>
@@ -1814,9 +1812,9 @@
         <v>7</v>
       </c>
       <c r="C59" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D59" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D59" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E59" t="s">
@@ -1826,7 +1824,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -1834,9 +1832,9 @@
         <v>7</v>
       </c>
       <c r="C60" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D60" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D60" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E60" t="s">
@@ -1846,7 +1844,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>69</v>
       </c>
@@ -1854,9 +1852,9 @@
         <v>7</v>
       </c>
       <c r="C61" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D61" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D61" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E61" t="s">
@@ -1866,7 +1864,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>70</v>
       </c>
@@ -1874,9 +1872,9 @@
         <v>7</v>
       </c>
       <c r="C62" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D62" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D62" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E62" t="s">
@@ -1886,7 +1884,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>71</v>
       </c>
@@ -1894,9 +1892,9 @@
         <v>7</v>
       </c>
       <c r="C63" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D63" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D63" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E63" t="s">
@@ -1906,7 +1904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>72</v>
       </c>
@@ -1914,9 +1912,9 @@
         <v>7</v>
       </c>
       <c r="C64" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D64" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D64" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E64" t="s">
@@ -1926,7 +1924,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>73</v>
       </c>
@@ -1934,9 +1932,9 @@
         <v>7</v>
       </c>
       <c r="C65" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D65" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D65" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E65" t="s">
@@ -1946,7 +1944,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>74</v>
       </c>
@@ -1954,9 +1952,9 @@
         <v>7</v>
       </c>
       <c r="C66" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D66" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D66" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E66" t="s">
@@ -1966,7 +1964,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>75</v>
       </c>
@@ -1974,9 +1972,9 @@
         <v>7</v>
       </c>
       <c r="C67" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D67" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D67" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E67" t="s">
@@ -1986,7 +1984,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>76</v>
       </c>
@@ -1994,9 +1992,9 @@
         <v>7</v>
       </c>
       <c r="C68" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D68" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D68" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E68" t="s">
@@ -2006,7 +2004,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>77</v>
       </c>
@@ -2014,9 +2012,9 @@
         <v>7</v>
       </c>
       <c r="C69" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D69" s="3">
+        <v>45906</v>
+      </c>
+      <c r="D69" s="2">
         <v>0.48561342592592593</v>
       </c>
       <c r="E69" t="s">

</xml_diff>